<commit_message>
Structured the project and sent it for review
</commit_message>
<xml_diff>
--- a/Lection 3/task 3.1/ReportApp/Templates/ActivityReport.xlsx
+++ b/Lection 3/task 3.1/ReportApp/Templates/ActivityReport.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F1B19B-5E57-47FD-B129-BB2651DEEE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="10650" yWindow="165" windowWidth="18120" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,111 +123,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -239,47 +141,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -289,57 +150,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -359,9 +186,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -399,9 +226,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,7 +298,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -644,137 +471,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="14" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="2" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="3" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>